<commit_message>
Activities & Contacts Module changes - 12 Feb 2023
</commit_message>
<xml_diff>
--- a/TestData/TMTT0005673_ActivitiesList_VerifyPreSetTemplateList.xlsx
+++ b/TestData/TMTT0005673_ActivitiesList_VerifyPreSetTemplateList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20393"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19018845-4498-4D05-B661-E13468D859CB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD9B5F2-058E-4CBD-AEC5-0EAC347D0EA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18420" windowHeight="6456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>StdUser</t>
   </si>
@@ -46,16 +46,19 @@
     <t>My Last 30 days Activities</t>
   </si>
   <si>
+    <t>My Activities Today</t>
+  </si>
+  <si>
+    <t>My Activities Tomorrow</t>
+  </si>
+  <si>
+    <t>My Activities Yesterday</t>
+  </si>
+  <si>
+    <t>My Last 100 days Activities</t>
+  </si>
+  <si>
     <t>Activities Filtered by Andrew B</t>
-  </si>
-  <si>
-    <t>My Activities Today</t>
-  </si>
-  <si>
-    <t>My Activities Tomorrow</t>
-  </si>
-  <si>
-    <t>My Activities Yesterday</t>
   </si>
 </sst>
 </file>
@@ -412,10 +415,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -433,36 +436,41 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changes - 29th feb 2024
</commit_message>
<xml_diff>
--- a/TestData/TMTT0005673_ActivitiesList_VerifyPreSetTemplateList.xlsx
+++ b/TestData/TMTT0005673_ActivitiesList_VerifyPreSetTemplateList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD9B5F2-058E-4CBD-AEC5-0EAC347D0EA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4313AE99-FF5E-4BDB-AB65-B8F59E9F6D57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -389,7 +389,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -418,7 +418,7 @@
   <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Activities Classic - 26 June
</commit_message>
<xml_diff>
--- a/TestData/TMTT0005673_ActivitiesList_VerifyPreSetTemplateList.xlsx
+++ b/TestData/TMTT0005673_ActivitiesList_VerifyPreSetTemplateList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4313AE99-FF5E-4BDB-AB65-B8F59E9F6D57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D36C73E4-350A-4A21-8236-03F73AECE46F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>StdUser</t>
   </si>
@@ -53,9 +53,6 @@
   </si>
   <si>
     <t>My Activities Yesterday</t>
-  </si>
-  <si>
-    <t>My Last 100 days Activities</t>
   </si>
   <si>
     <t>Activities Filtered by Andrew B</t>
@@ -102,10 +99,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,10 +411,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -435,8 +431,8 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>10</v>
+      <c r="A2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
@@ -456,21 +452,16 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>